<commit_message>
upload of excel file
</commit_message>
<xml_diff>
--- a/test_excel.xlsx
+++ b/test_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RCrystalOrnelas/Desktop/research/github-systematic-review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE4B0BE1-002E-F84F-A861-8BB4400466CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2BAD5D-7188-414D-AD73-AE021963A96F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30860" yWindow="3380" windowWidth="28040" windowHeight="15880" xr2:uid="{60043A13-9FE4-8243-85B6-2635F4E92CFA}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Test column A</t>
   </si>
   <si>
     <t>Test column b</t>
+  </si>
+  <si>
+    <t>Test column c</t>
   </si>
 </sst>
 </file>
@@ -382,19 +385,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D8673B-B740-134A-B880-1049047E41A6}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>